<commit_message>
fixed problem with correct_names_tree dictionary
Signed-off-by: Nelson Buainain <nnbuainain@gmail.com>
</commit_message>
<xml_diff>
--- a/correct_names_tree_py/dict_correct_names.xlsx
+++ b/correct_names_tree_py/dict_correct_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nnbuainain/Dropbox/Data_Science/Projects/get_confidence_interval_from_treePL/correct_names_tree_PY/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70ED2BC4-792A-3E41-AB95-DED89E9C7CED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD61F47A-5663-BA40-A894-6CFFE125ACCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="540" yWindow="540" windowWidth="24940" windowHeight="14200" xr2:uid="{9D80F51E-49F9-CD46-9FB8-A2C03BB9411C}"/>
   </bookViews>
@@ -102,6 +102,9 @@
     <t>LSU_66929_Arr_abe_abe_allele1</t>
   </si>
   <si>
+    <t>Andes_O_221_Arr_tac_axi_allele1</t>
+  </si>
+  <si>
     <t>LSU_66257_Arr_aur_san_allele1</t>
   </si>
   <si>
@@ -586,9 +589,6 @@
   </si>
   <si>
     <t>nome_final</t>
-  </si>
-  <si>
-    <t>Andes_O_221_Arr_tac_axi_allele1,</t>
   </si>
 </sst>
 </file>
@@ -944,7 +944,7 @@
   <dimension ref="A1:B94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="A1:B94"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -955,82 +955,82 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1038,31 +1038,31 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>187</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1070,23 +1070,23 @@
         <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1094,31 +1094,31 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1126,31 +1126,31 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1158,103 +1158,103 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1262,15 +1262,15 @@
         <v>10</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1278,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1286,15 +1286,15 @@
         <v>13</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1302,7 +1302,7 @@
         <v>1</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1310,23 +1310,23 @@
         <v>23</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1334,47 +1334,47 @@
         <v>11</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1382,15 +1382,15 @@
         <v>21</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1398,15 +1398,15 @@
         <v>24</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1414,31 +1414,31 @@
         <v>6</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1446,15 +1446,15 @@
         <v>12</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1462,55 +1462,55 @@
         <v>19</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1518,15 +1518,15 @@
         <v>18</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1542,15 +1542,15 @@
         <v>17</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1558,7 +1558,7 @@
         <v>15</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1566,31 +1566,31 @@
         <v>9</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1598,63 +1598,63 @@
         <v>2</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1662,7 +1662,7 @@
         <v>4</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1670,7 +1670,7 @@
         <v>8</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1678,31 +1678,31 @@
         <v>14</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>